<commit_message>
update AE for Modbus
</commit_message>
<xml_diff>
--- a/sanjay/Modbus Regs.xlsx
+++ b/sanjay/Modbus Regs.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t xml:space="preserve">Sr. No. </t>
   </si>
@@ -582,12 +582,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -615,6 +609,12 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -935,7 +935,7 @@
   <dimension ref="C4:N54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -960,12 +960,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" ht="15">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
     </row>
     <row r="5" spans="3:10" ht="15">
       <c r="C5" s="2"/>
@@ -974,12 +974,12 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="3:10" ht="15">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="3:10" ht="15.75" thickBot="1">
       <c r="C7" s="2"/>
@@ -1176,12 +1176,12 @@
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="3:11" ht="15">
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="3:11" ht="15.75" thickBot="1">
       <c r="C25" s="2"/>
@@ -1388,12 +1388,12 @@
       <c r="F41" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H41" s="14" t="s">
+      <c r="H41" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
     </row>
     <row r="42" spans="3:11">
       <c r="C42" s="8">
@@ -1409,6 +1409,9 @@
       <c r="H43" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="J43" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="46" spans="3:11">
       <c r="H46" s="1" t="s">
@@ -1442,58 +1445,58 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="8:14" ht="36">
-      <c r="L50" s="16" t="s">
+    <row r="50" spans="8:14" ht="18">
+      <c r="L50" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="M50" s="17" t="s">
+      <c r="M50" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="N50" s="18" t="s">
+      <c r="N50" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="8:14" ht="36">
-      <c r="L51" s="19" t="s">
+    <row r="51" spans="8:14" ht="18">
+      <c r="L51" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="M51" s="15" t="s">
+      <c r="M51" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="N51" s="20" t="s">
+      <c r="N51" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="52" spans="8:14" ht="36">
-      <c r="L52" s="19" t="s">
+      <c r="L52" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="M52" s="15" t="s">
+      <c r="M52" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="N52" s="20" t="s">
+      <c r="N52" s="16" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="53" spans="8:14" ht="36">
-      <c r="L53" s="19" t="s">
+      <c r="L53" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="M53" s="15" t="s">
+      <c r="M53" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="N53" s="20" t="s">
+      <c r="N53" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="54" spans="8:14" ht="36.75" thickBot="1">
-      <c r="L54" s="21" t="s">
+      <c r="L54" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="M54" s="22" t="s">
+      <c r="M54" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="N54" s="23" t="s">
+      <c r="N54" s="19" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated for UP and Down Movement
</commit_message>
<xml_diff>
--- a/sanjay/Modbus Regs.xlsx
+++ b/sanjay/Modbus Regs.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
   <si>
     <t xml:space="preserve">Sr. No. </t>
   </si>
@@ -275,6 +275,15 @@
   </si>
   <si>
     <t>DOWN</t>
+  </si>
+  <si>
+    <t>0:Ext</t>
+  </si>
+  <si>
+    <t>1:Encoder</t>
+  </si>
+  <si>
+    <t>1=Stop</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -587,6 +596,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -594,7 +616,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -603,9 +625,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -639,6 +659,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -959,7 +983,7 @@
   <dimension ref="C4:N58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -984,12 +1008,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" ht="15">
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="3:10" ht="15">
       <c r="C5" s="2"/>
@@ -998,12 +1022,12 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="3:10" ht="15">
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="3:10" ht="15.75" thickBot="1">
       <c r="C7" s="2"/>
@@ -1138,66 +1162,66 @@
       </c>
     </row>
     <row r="17" spans="3:11" ht="15">
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>9</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" spans="3:11" ht="15">
-      <c r="C18" s="7">
+      <c r="C18" s="4">
         <v>10</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="3:11" ht="15">
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>11</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" spans="3:11" ht="15">
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>12</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="3:11" ht="15">
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>13</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="4" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1238,12 +1262,12 @@
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="3:11" ht="15">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="3:11" ht="15.75" thickBot="1">
       <c r="C29" s="2"/>
@@ -1384,17 +1408,23 @@
       </c>
     </row>
     <row r="39" spans="3:11" ht="15">
-      <c r="C39" s="7">
+      <c r="C39" s="4">
         <v>9</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="7">
-        <v>1</v>
-      </c>
-      <c r="F39" s="7" t="s">
+      <c r="E39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>55</v>
+      </c>
+      <c r="I39" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="3:11" ht="15">
@@ -1429,21 +1459,21 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="3:11" ht="16.5" thickTop="1" thickBot="1">
-      <c r="C44" s="3" t="s">
+    <row r="44" spans="3:11" ht="15.75" thickTop="1">
+      <c r="C44" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F44" s="25" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="3:11" ht="16.5" thickTop="1">
+    <row r="45" spans="3:11" ht="15.75">
       <c r="C45" s="4">
         <v>1</v>
       </c>
@@ -1456,32 +1486,39 @@
       <c r="F45" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
     </row>
     <row r="46" spans="3:11">
-      <c r="C46" s="8">
+      <c r="C46" s="23">
         <v>2</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
+      <c r="E46" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="24"/>
+      <c r="H46" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="47" spans="3:11">
-      <c r="C47" s="9">
+      <c r="C47" s="23">
         <v>3</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
+      <c r="E47" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" s="23"/>
       <c r="H47" s="1" t="s">
         <v>42</v>
       </c>
@@ -1490,16 +1527,28 @@
       </c>
     </row>
     <row r="48" spans="3:11">
-      <c r="C48" s="9">
+      <c r="C48" s="23">
         <v>4</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-    </row>
-    <row r="50" spans="8:14">
+      <c r="E48" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F48" s="23"/>
+    </row>
+    <row r="49" spans="3:14">
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+    </row>
+    <row r="50" spans="3:14">
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
       <c r="H50" s="1" t="s">
         <v>43</v>
       </c>
@@ -1507,7 +1556,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="8:14">
+    <row r="51" spans="3:14">
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
       <c r="H51" s="1">
         <v>1</v>
       </c>
@@ -1515,7 +1568,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="8:14">
+    <row r="52" spans="3:14">
       <c r="H52" s="1">
         <v>0</v>
       </c>
@@ -1523,66 +1576,66 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="8:14" ht="15" thickBot="1">
-      <c r="H53" s="9">
+    <row r="53" spans="3:14" ht="15" thickBot="1">
+      <c r="H53" s="8">
         <v>2</v>
       </c>
-      <c r="I53" s="9" t="s">
+      <c r="I53" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="8:14" ht="18">
-      <c r="L54" s="12" t="s">
+    <row r="54" spans="3:14" ht="18">
+      <c r="L54" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="M54" s="13" t="s">
+      <c r="M54" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="N54" s="14" t="s">
+      <c r="N54" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="8:14" ht="18">
-      <c r="L55" s="15" t="s">
+    <row r="55" spans="3:14" ht="18">
+      <c r="L55" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="M55" s="11" t="s">
+      <c r="M55" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="N55" s="16" t="s">
+      <c r="N55" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="8:14" ht="36">
-      <c r="L56" s="15" t="s">
+    <row r="56" spans="3:14" ht="36">
+      <c r="L56" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="M56" s="11" t="s">
+      <c r="M56" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="N56" s="16" t="s">
+      <c r="N56" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="8:14" ht="36">
-      <c r="L57" s="15" t="s">
+    <row r="57" spans="3:14" ht="36">
+      <c r="L57" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="M57" s="11" t="s">
+      <c r="M57" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="N57" s="16" t="s">
+      <c r="N57" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="8:14" ht="36.75" thickBot="1">
-      <c r="L58" s="17" t="s">
+    <row r="58" spans="3:14" ht="36.75" thickBot="1">
+      <c r="L58" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="M58" s="18" t="s">
+      <c r="M58" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="N58" s="19" t="s">
+      <c r="N58" s="17" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>